<commit_message>
Rodzial o czasie poajwiania sie regeneratow na esk0pantatach
</commit_message>
<xml_diff>
--- a/Ilosc eksplantatow ktora podjela rozwoj oraz czas.xlsx
+++ b/Ilosc eksplantatow ktora podjela rozwoj oraz czas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E05EB4-EF06-447E-85B6-42FD3F2E7ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D388E8BE-6459-4988-8AA3-086A284A6635}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,26 +16,6 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Baza danych - sniezyca'!$A$1:$T$100</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Baza danych - szachownica'!$A$1:$Q$65</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'Ilosc ekspl z rozwoj '!$A$4:$A$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Ilosc ekspl z rozwoj '!$A$8:$A$12</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Ilosc ekspl z rozwoj '!$A$4:$A$7</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Ilosc ekspl z rozwoj '!$A$8:$A$12</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Ilosc ekspl z rozwoj '!$B$3:$B$7</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Ilosc ekspl z rozwoj '!$E$3:$E$7</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Ilosc ekspl z rozwoj '!$E$8:$E$12</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Ilosc ekspl z rozwoj '!$A$4:$A$7</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Ilosc ekspl z rozwoj '!$A$8:$A$12</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Ilosc ekspl z rozwoj '!$B$3:$B$7</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Ilosc ekspl z rozwoj '!$E$3:$E$7</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Ilosc ekspl z rozwoj '!$E$8:$E$12</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Ilosc ekspl z rozwoj '!$B$3:$B$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Ilosc ekspl z rozwoj '!$E$3:$E$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Ilosc ekspl z rozwoj '!$E$8:$E$12</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Ilosc ekspl z rozwoj '!$A$4:$A$7</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Ilosc ekspl z rozwoj '!$A$8:$A$12</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Ilosc ekspl z rozwoj '!$B$3:$B$7</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Ilosc ekspl z rozwoj '!$E$3:$E$7</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Ilosc ekspl z rozwoj '!$E$8:$E$12</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -53,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="258">
   <si>
     <t>Nazwa gatunkowa</t>
   </si>
@@ -703,9 +683,6 @@
     <t>6 kwietnia</t>
   </si>
   <si>
-    <t>Sniezyca karpacka</t>
-  </si>
-  <si>
     <t>25 maja</t>
   </si>
   <si>
@@ -727,9 +704,6 @@
     <t>11-15 dni</t>
   </si>
   <si>
-    <t>około tygodnia</t>
-  </si>
-  <si>
     <t>około 2 tygodni</t>
   </si>
   <si>
@@ -769,62 +743,138 @@
     <t>około 9 tygodni</t>
   </si>
   <si>
-    <t>Liczba tygodni</t>
-  </si>
-  <si>
-    <t>około 1</t>
-  </si>
-  <si>
-    <t>około 2</t>
-  </si>
-  <si>
-    <t>około 3</t>
-  </si>
-  <si>
-    <t>około 4</t>
-  </si>
-  <si>
-    <t>około 5</t>
-  </si>
-  <si>
-    <t>około 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">około 7 </t>
-  </si>
-  <si>
-    <t>około 8</t>
-  </si>
-  <si>
-    <t>około 9</t>
-  </si>
-  <si>
-    <t>przysorst</t>
-  </si>
-  <si>
     <t>sniezyca karpacka</t>
   </si>
   <si>
-    <t>łuska</t>
-  </si>
-  <si>
-    <t>piętka</t>
-  </si>
-  <si>
     <t>szachownica kostkowata</t>
   </si>
   <si>
-    <t>pietka</t>
-  </si>
-  <si>
-    <t>Suma</t>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Leucojum vernum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> var. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>carpathicum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sweet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fritillaria meleagris</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> L.</t>
+    </r>
+  </si>
+  <si>
+    <t>Data założenia kultury</t>
+  </si>
+  <si>
+    <t>Data obserwacji</t>
+  </si>
+  <si>
+    <t>śniezyca karpacka</t>
+  </si>
+  <si>
+    <t>około 1 tygodnia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unikalna wartość z </t>
+  </si>
+  <si>
+    <t>Zakresy przyjętych pdzedziałów</t>
+  </si>
+  <si>
+    <t>Nazwy przyjętych przedziałów</t>
+  </si>
+  <si>
+    <t>Przedział obserwacji</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>VII</t>
+  </si>
+  <si>
+    <t>VIII</t>
+  </si>
+  <si>
+    <t>IX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suma </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +898,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -857,7 +915,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -932,11 +990,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1017,17 +1130,38 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1044,44 +1178,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,7 +1276,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL" b="1" i="0" cap="none" baseline="0"/>
-              <a:t>Udział eskplantatow które podjęły regenerację</a:t>
+              <a:t>Ilość eksplantatów która podjęła rozwój</a:t>
             </a:r>
             <a:endParaRPr lang="pl-PL" b="0" i="0" cap="none" baseline="0"/>
           </a:p>
@@ -1186,7 +1327,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Śnieżyca karpacka</c:v>
+                  <c:v>Leucojum vernum var. carpathicum Sweet</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1320,7 +1461,7 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Szachownica kostkowata</c:v>
+                  <c:v>Fritillaria meleagris L.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1723,8 +1864,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="pl-PL" b="1" i="1" cap="none" baseline="0"/>
+              <a:t>Leucojum vernum </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="pl-PL" b="1" i="0" cap="none" baseline="0"/>
-              <a:t>sniezyca karpacka</a:t>
+              <a:t>var. </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" b="1" i="1" cap="none" baseline="0"/>
+              <a:t>carpathicum</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" b="1" i="0" cap="none" baseline="0"/>
+              <a:t> Sweet</a:t>
             </a:r>
             <a:endParaRPr lang="pl-PL" b="0" i="0" cap="none" baseline="0"/>
           </a:p>
@@ -1773,9 +1926,9 @@
             <c:strRef>
               <c:f>'Ilosc eksplanta a czas'!$N$34:$N$35</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>łuska</c:v>
+                  <c:v>Łuska</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1853,31 +2006,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>około 1</c:v>
+                  <c:v>I</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>około 2</c:v>
+                  <c:v>II</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>około 3</c:v>
+                  <c:v>III</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>około 4</c:v>
+                  <c:v>IV</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>około 5</c:v>
+                  <c:v>V</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>około 6</c:v>
+                  <c:v>VI</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>około 7 </c:v>
+                  <c:v>VII</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>około 8</c:v>
+                  <c:v>VIII</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>około 9</c:v>
+                  <c:v>IX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1931,9 +2084,9 @@
             <c:strRef>
               <c:f>'Ilosc eksplanta a czas'!$N$36:$N$37</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>piętka</c:v>
+                  <c:v>Piętka</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2011,31 +2164,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>około 1</c:v>
+                  <c:v>I</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>około 2</c:v>
+                  <c:v>II</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>około 3</c:v>
+                  <c:v>III</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>około 4</c:v>
+                  <c:v>IV</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>około 5</c:v>
+                  <c:v>V</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>około 6</c:v>
+                  <c:v>VI</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>około 7 </c:v>
+                  <c:v>VII</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>około 8</c:v>
+                  <c:v>VIII</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>około 9</c:v>
+                  <c:v>IX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2360,8 +2513,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="pl-PL" b="1" i="1" cap="none" baseline="0"/>
+              <a:t>Fritillaria meleagris </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="pl-PL" b="1" i="0" cap="none" baseline="0"/>
-              <a:t>szachownica kostkowata</a:t>
+              <a:t>L.</a:t>
             </a:r>
             <a:endParaRPr lang="pl-PL" b="0" i="0" cap="none" baseline="0"/>
           </a:p>
@@ -2412,7 +2569,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>łuska</c:v>
+                  <c:v>Łuska</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2490,31 +2647,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>około 1</c:v>
+                  <c:v>I</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>około 2</c:v>
+                  <c:v>II</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>około 3</c:v>
+                  <c:v>III</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>około 4</c:v>
+                  <c:v>IV</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>około 5</c:v>
+                  <c:v>V</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>około 6</c:v>
+                  <c:v>VI</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>około 7 </c:v>
+                  <c:v>VII</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>około 8</c:v>
+                  <c:v>VIII</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>około 9</c:v>
+                  <c:v>IX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2570,7 +2727,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pietka</c:v>
+                  <c:v>Piętka</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2648,31 +2805,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>około 1</c:v>
+                  <c:v>I</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>około 2</c:v>
+                  <c:v>II</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>około 3</c:v>
+                  <c:v>III</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>około 4</c:v>
+                  <c:v>IV</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>około 5</c:v>
+                  <c:v>V</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>około 6</c:v>
+                  <c:v>VI</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>około 7 </c:v>
+                  <c:v>VII</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>około 8</c:v>
+                  <c:v>VIII</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>około 9</c:v>
+                  <c:v>IX</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5185,64 +5342,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="30" t="s">
+      <c r="I1" s="36"/>
+      <c r="J1" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="30" t="s">
+      <c r="K1" s="36"/>
+      <c r="L1" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="30" t="s">
+      <c r="M1" s="36"/>
+      <c r="N1" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="30" t="s">
+      <c r="O1" s="36"/>
+      <c r="P1" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="30" t="s">
+      <c r="Q1" s="36"/>
+      <c r="R1" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="S1" s="31"/>
-      <c r="T1" s="28" t="s">
+      <c r="S1" s="36"/>
+      <c r="T1" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="U1" s="28"/>
+      <c r="U1" s="37"/>
     </row>
     <row r="2" spans="1:21" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="3" t="s">
         <v>105</v>
       </c>
@@ -11677,6 +11834,13 @@
     <filterColumn colId="19" showButton="0"/>
   </autoFilter>
   <mergeCells count="14">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
@@ -11684,13 +11848,6 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11723,56 +11880,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="30" t="s">
+      <c r="I1" s="36"/>
+      <c r="J1" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="30" t="s">
+      <c r="K1" s="36"/>
+      <c r="L1" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="30" t="s">
+      <c r="M1" s="36"/>
+      <c r="N1" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="30" t="s">
+      <c r="O1" s="36"/>
+      <c r="P1" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="Q1" s="31"/>
+      <c r="Q1" s="36"/>
     </row>
     <row r="2" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
       <c r="H2" s="13" t="s">
         <v>105</v>
       </c>
@@ -15050,6 +15207,11 @@
     <filterColumn colId="15" showButton="0"/>
   </autoFilter>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="F1:F2"/>
@@ -15057,11 +15219,6 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15072,7 +15229,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15085,26 +15242,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="29"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="36"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="15" t="s">
         <v>206</v>
       </c>
@@ -15132,8 +15289,8 @@
       <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>201</v>
+      <c r="A4" s="47" t="s">
+        <v>238</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>202</v>
@@ -15152,7 +15309,7 @@
       <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="22" t="s">
         <v>204</v>
       </c>
@@ -15169,7 +15326,7 @@
       <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
@@ -15187,7 +15344,7 @@
       <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
@@ -15205,8 +15362,8 @@
       <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>52</v>
+      <c r="A8" s="39" t="s">
+        <v>239</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>203</v>
@@ -15225,7 +15382,7 @@
       <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="4" t="s">
         <v>202</v>
       </c>
@@ -15243,7 +15400,7 @@
       <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="4" t="s">
         <v>204</v>
       </c>
@@ -15261,7 +15418,7 @@
       <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
@@ -15279,7 +15436,7 @@
       <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
@@ -15315,8 +15472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8DFBC29-382F-40AB-8DFA-A6A0286E4B26}">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="H61" workbookViewId="0">
+      <selection activeCell="Z50" sqref="Z50:Z51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15340,26 +15497,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="29"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="36"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="19" t="s">
         <v>206</v>
       </c>
@@ -15370,7 +15527,7 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="39" t="s">
         <v>201</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -15390,7 +15547,7 @@
       <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="22" t="s">
         <v>28</v>
       </c>
@@ -15408,7 +15565,7 @@
       <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="22" t="s">
         <v>29</v>
       </c>
@@ -15426,7 +15583,7 @@
       <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="39" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="22" t="s">
@@ -15446,7 +15603,7 @@
       <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="22" t="s">
         <v>202</v>
       </c>
@@ -15464,7 +15621,7 @@
       <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="22" t="s">
         <v>204</v>
       </c>
@@ -15482,7 +15639,7 @@
       <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="22" t="s">
         <v>28</v>
       </c>
@@ -15500,7 +15657,7 @@
       <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="22" t="s">
         <v>29</v>
       </c>
@@ -15517,199 +15674,214 @@
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25" t="s">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="48"/>
+      <c r="C18" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="I19" s="28" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="C20" s="38">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" s="30">
         <v>8</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="30">
         <v>15</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="30">
         <v>29</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="30">
         <v>39</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="30">
         <v>43</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="30">
         <v>50</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="30">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="38" t="s">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="39"/>
+      <c r="B21" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="38">
+      <c r="C21" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="30">
         <v>8</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="30">
         <v>22</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="30">
         <v>32</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="30">
         <v>36</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="28">
         <v>43</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="28">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="38" t="s">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="39"/>
+      <c r="B22" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="C22" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="38">
+      <c r="C22" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="30">
         <v>15</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="30">
         <v>25</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="30">
         <v>29</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="28">
         <v>36</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="28">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="39"/>
+      <c r="B23" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="C23" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="38">
+      <c r="C23" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="30">
         <v>11</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="30">
         <v>15</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="28">
         <v>22</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="28">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="38" t="s">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="39"/>
+      <c r="B24" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="C24" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="G24" s="38">
-        <v>5</v>
-      </c>
-      <c r="H24" s="25">
+      <c r="C24" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="30">
+        <v>5</v>
+      </c>
+      <c r="H24" s="28">
         <v>12</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="28">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="s">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="H25" s="45">
+      <c r="C25" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="32">
         <v>8</v>
       </c>
-      <c r="I25" s="45">
+      <c r="I25" s="32">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -15719,158 +15891,165 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="25" t="s">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
-      <c r="C28" s="25" t="s">
+      <c r="B27" s="48"/>
+      <c r="C27" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="G28" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="G28" s="25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="25" t="s">
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="38">
-        <v>5</v>
-      </c>
-      <c r="D29" s="25">
+      <c r="C29" s="30">
+        <v>5</v>
+      </c>
+      <c r="D29" s="28">
         <v>12</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="28">
         <v>26</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="28">
         <v>40</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="28">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="25" t="s">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="39"/>
+      <c r="B30" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="25">
+      <c r="C30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="28">
         <v>15</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="28">
         <v>29</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="28">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="s">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="39"/>
+      <c r="B31" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="C31" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31" s="25">
+      <c r="C31" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="28">
         <v>15</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="28">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="40"/>
-      <c r="S32" s="40"/>
-      <c r="T32" s="40"/>
-      <c r="U32" s="40"/>
-      <c r="V32" s="40"/>
-      <c r="W32" s="40"/>
-      <c r="X32" s="43" t="s">
-        <v>254</v>
+      <c r="M32" s="56"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="48"/>
+      <c r="T32" s="48"/>
+      <c r="U32" s="48"/>
+      <c r="V32" s="48"/>
+      <c r="W32" s="48"/>
+      <c r="X32" s="46" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="59"/>
       <c r="O33" s="25" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="P33" s="25" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="Q33" s="25" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="R33" s="25" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="S33" s="25" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="T33" s="25" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="U33" s="25" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="W33" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="X33" s="43"/>
+        <v>256</v>
+      </c>
+      <c r="X33" s="46"/>
     </row>
     <row r="34" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L34" s="32" t="s">
-        <v>248</v>
-      </c>
-      <c r="M34" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="N34" s="41" t="s">
-        <v>250</v>
+      <c r="L34" s="39"/>
+      <c r="M34" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="N34" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="O34" s="25">
         <v>0</v>
@@ -15899,15 +16078,15 @@
       <c r="W34" s="25">
         <v>0</v>
       </c>
-      <c r="X34" s="32">
+      <c r="X34" s="39">
         <f>SUM(O34:W34)</f>
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L35" s="32"/>
-      <c r="M35" s="41"/>
-      <c r="N35" s="41"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
       <c r="O35" s="24">
         <f>O34*100/$X$34</f>
         <v>0</v>
@@ -15944,103 +16123,103 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X35" s="32"/>
+      <c r="X35" s="39"/>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="L36" s="32"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="O36" s="46">
+      <c r="L36" s="39"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="O36" s="33">
         <v>33</v>
       </c>
-      <c r="P36" s="46">
+      <c r="P36" s="33">
         <v>22</v>
       </c>
-      <c r="Q36" s="46">
+      <c r="Q36" s="33">
         <v>10</v>
       </c>
-      <c r="R36" s="46">
+      <c r="R36" s="33">
         <v>3</v>
       </c>
-      <c r="S36" s="46">
+      <c r="S36" s="33">
         <v>9</v>
       </c>
-      <c r="T36" s="46">
+      <c r="T36" s="33">
         <v>3</v>
       </c>
-      <c r="U36" s="46">
+      <c r="U36" s="33">
         <v>1</v>
       </c>
-      <c r="V36" s="46">
-        <v>0</v>
-      </c>
-      <c r="W36" s="46">
-        <v>0</v>
-      </c>
-      <c r="X36" s="32">
+      <c r="V36" s="33">
+        <v>0</v>
+      </c>
+      <c r="W36" s="33">
+        <v>0</v>
+      </c>
+      <c r="X36" s="39">
         <f>SUM(O36:W36)</f>
         <v>81</v>
       </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="L37" s="32"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="49">
+      <c r="L37" s="39"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="34">
         <f>O36*100/$X$36</f>
         <v>40.74074074074074</v>
       </c>
-      <c r="P37" s="49">
+      <c r="P37" s="34">
         <f t="shared" ref="P37:W37" si="2">P36*100/$X$36</f>
         <v>27.160493827160494</v>
       </c>
-      <c r="Q37" s="49">
+      <c r="Q37" s="34">
         <f t="shared" si="2"/>
         <v>12.345679012345679</v>
       </c>
-      <c r="R37" s="49">
+      <c r="R37" s="34">
         <f t="shared" si="2"/>
         <v>3.7037037037037037</v>
       </c>
-      <c r="S37" s="49">
+      <c r="S37" s="34">
         <f t="shared" si="2"/>
         <v>11.111111111111111</v>
       </c>
-      <c r="T37" s="49">
+      <c r="T37" s="34">
         <f t="shared" si="2"/>
         <v>3.7037037037037037</v>
       </c>
-      <c r="U37" s="49">
+      <c r="U37" s="34">
         <f t="shared" si="2"/>
         <v>1.2345679012345678</v>
       </c>
-      <c r="V37" s="49">
+      <c r="V37" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W37" s="49">
+      <c r="W37" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X37" s="32"/>
+      <c r="X37" s="39"/>
     </row>
     <row r="38" spans="2:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="N38" s="32" t="s">
-        <v>250</v>
+      <c r="L38" s="39"/>
+      <c r="M38" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="N38" s="39" t="s">
+        <v>28</v>
       </c>
       <c r="O38" s="25">
         <v>0</v>
@@ -16069,7 +16248,7 @@
       <c r="W38" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="X38" s="47">
+      <c r="X38" s="44">
         <f>SUM(O38:W38)</f>
         <v>55</v>
       </c>
@@ -16077,19 +16256,16 @@
     <row r="39" spans="2:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="16"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="42"/>
-      <c r="N39" s="32"/>
+      <c r="D39" s="54"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="39"/>
       <c r="O39" s="24">
         <f>O38*100/$X$38</f>
         <v>0</v>
       </c>
       <c r="P39" s="24">
-        <f t="shared" ref="P39:W39" si="3">P38*100/$X$38</f>
+        <f t="shared" ref="P39:V39" si="3">P38*100/$X$38</f>
         <v>7.2727272727272725</v>
       </c>
       <c r="Q39" s="24" t="s">
@@ -16116,15 +16292,24 @@
       <c r="W39" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="X39" s="48"/>
-    </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="X39" s="45"/>
+    </row>
+    <row r="40" spans="2:24" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="32" t="s">
-        <v>253</v>
+      <c r="E40" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F40" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="G40" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="L40" s="39"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="O40" s="25">
         <v>3</v>
@@ -16153,7 +16338,7 @@
       <c r="W40" s="25">
         <v>0</v>
       </c>
-      <c r="X40" s="47">
+      <c r="X40" s="44">
         <f>SUM(O40:W40)</f>
         <v>16</v>
       </c>
@@ -16161,19 +16346,18 @@
     <row r="41" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="5">
-        <v>5</v>
-      </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="L41" s="32"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="32"/>
+      <c r="E41" s="28">
+        <v>5</v>
+      </c>
+      <c r="F41" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="L41" s="39"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="39"/>
       <c r="O41" s="24">
         <f>O40*100/$X$40</f>
         <v>18.75</v>
@@ -16207,212 +16391,227 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X41" s="48"/>
+      <c r="X41" s="45"/>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="5">
+      <c r="E42" s="28">
         <v>8</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="45"/>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="5">
+      <c r="E43" s="28">
         <v>11</v>
       </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="G43" s="44" t="s">
         <v>223</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="5">
+      <c r="E44" s="28">
         <v>12</v>
       </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="5">
+      <c r="E45" s="28">
         <v>15</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
     </row>
     <row r="46" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="5">
+      <c r="E46" s="28">
         <v>22</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>226</v>
+      <c r="F46" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="G46" s="44" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="5">
+      <c r="E47" s="28">
         <v>25</v>
       </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="45"/>
     </row>
     <row r="48" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="5">
+      <c r="E48" s="28">
         <v>26</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>232</v>
+      <c r="F48" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="G48" s="44" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="5">
+      <c r="E49" s="28">
         <v>29</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="5">
+      <c r="E50" s="28">
         <v>32</v>
       </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>233</v>
+      <c r="F50" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="5">
+      <c r="E51" s="28">
         <v>36</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="5">
+      <c r="E52" s="28">
         <v>39</v>
       </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>234</v>
+      <c r="F52" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="G52" s="44" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
-      <c r="D53" s="5">
+      <c r="E53" s="28">
         <v>40</v>
       </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
-      <c r="D54" s="5">
+      <c r="E54" s="28">
         <v>43</v>
       </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
-      <c r="D55" s="5">
+      <c r="E55" s="28">
         <v>50</v>
       </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5">
+      <c r="F55" s="28">
         <v>50</v>
       </c>
-      <c r="G55" s="5" t="s">
-        <v>235</v>
+      <c r="G55" s="28" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
-      <c r="D56" s="5">
+      <c r="E56" s="28">
         <v>57</v>
       </c>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5">
+      <c r="F56" s="28">
         <v>57</v>
       </c>
-      <c r="G56" s="5" t="s">
-        <v>236</v>
+      <c r="G56" s="28" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
-      <c r="D57" s="5">
+      <c r="E57" s="28">
         <v>64</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>237</v>
+      <c r="F57" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="5">
+      <c r="E58" s="28">
         <v>65</v>
       </c>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="40">
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="O32:W32"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="M38:M41"/>
+    <mergeCell ref="L34:L41"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
     <mergeCell ref="X38:X39"/>
     <mergeCell ref="X40:X41"/>
     <mergeCell ref="X32:X33"/>
@@ -16421,17 +16620,6 @@
     <mergeCell ref="N36:N37"/>
     <mergeCell ref="X34:X35"/>
     <mergeCell ref="X36:X37"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="O32:W32"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="M38:M41"/>
-    <mergeCell ref="L34:L41"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>